<commit_message>
Implemented support for pie charts (including 3D and doughnuts), updated documentation.
This is still limited to only pie and line charts, but I think that it is enough to release. I documented the limitation.

Closes #4.
</commit_message>
<xml_diff>
--- a/db2xls-bundle/sample/countries_template.xlsx
+++ b/db2xls-bundle/sample/countries_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\IdeaProjects\xls-utils\db2xls\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\IdeaProjects\xls-utils\db2xls-bundle\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6826D5CD-FAA7-4B5B-AA46-840B1DC4E7A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A7D623-1BEC-4AF2-A8F9-FEEF8CAF6860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E6806242-FA56-4FF9-82FC-D7F9366448D9}"/>
   </bookViews>
@@ -55,10 +55,10 @@
     <t>X</t>
   </si>
   <si>
-    <t>Countries by Size</t>
+    <t>Size (sqkm)</t>
   </si>
   <si>
-    <t>Size (sqkm)</t>
+    <t>Countries by Area</t>
   </si>
 </sst>
 </file>
@@ -120,6 +120,1631 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Top 10 Population</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Results!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A533-421D-99D1-2CA5FD0FBF0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Top 10 Area</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Results!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-499C-405C-BB60-395666606732}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>280987</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0710B8F-69CB-4652-B46A-4F25EC1C6DCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72F13F5F-CDFA-46CF-A3B8-4FFF00F1A417}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,7 +2108,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +2125,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -514,7 +2139,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -534,9 +2159,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>